<commit_message>
🚧 (chapter7): Review WIP
</commit_message>
<xml_diff>
--- a/dissertation/designs/Heuristic Consolidation.xlsx
+++ b/dissertation/designs/Heuristic Consolidation.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arneschreuder/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arneschreuder/Development/personal/masters.ai/dissertation/designs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CADDDEE-BF0F-4E4A-8EDD-04CFA83A4657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6C019C-9CFD-7442-B847-2C68B05AF811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{6DFA7F91-D994-1E45-B9E7-F07B16B402EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{6DFA7F91-D994-1E45-B9E7-F07B16B402EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">Sheet3!$A$1:$M$14</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="127">
   <si>
     <t>Heuristic Consolidation</t>
   </si>
@@ -348,6 +352,93 @@
   </si>
   <si>
     <t>1x30x15</t>
+  </si>
+  <si>
+    <t>Is analogous to the negative gradient</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>sgd</t>
+  </si>
+  <si>
+    <t>momentum</t>
+  </si>
+  <si>
+    <t>nag</t>
+  </si>
+  <si>
+    <t>adagrad</t>
+  </si>
+  <si>
+    <t>rmsprop</t>
+  </si>
+  <si>
+    <t>adadelta</t>
+  </si>
+  <si>
+    <t>adam</t>
+  </si>
+  <si>
+    <t>sum of gradients squared</t>
+  </si>
+  <si>
+    <t>expected position delta variance</t>
+  </si>
+  <si>
+    <t>learning rate</t>
+  </si>
+  <si>
+    <t>learning rate, epsilon</t>
+  </si>
+  <si>
+    <t>mutation rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">burn in, replay window size, population size, reselection and reanalysis window size, normalisation, discounted rewards  </t>
+  </si>
+  <si>
+    <t>Population State</t>
+  </si>
+  <si>
+    <t>heuristic</t>
+  </si>
+  <si>
+    <t>hyper-parameter</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Represents the candidate solution</t>
+  </si>
+  <si>
+    <t>Is analogous to velocity</t>
+  </si>
+  <si>
+    <t>learning rate, momentum (maps to hp1)</t>
+  </si>
+  <si>
+    <t>expected gradient mean (hp1)</t>
+  </si>
+  <si>
+    <t>expected gradient variance (hp2)</t>
+  </si>
+  <si>
+    <t>learning rate, rho  (maps to hp2), momentum (maps to hp1), epsilon</t>
+  </si>
+  <si>
+    <t>rho (maps to hp2), epsilon</t>
+  </si>
+  <si>
+    <t>learning rate, momentum (maps to hp1), rho (maps to hp2)</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -456,7 +547,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -479,11 +570,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -516,15 +616,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -536,13 +639,84 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -935,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E850A184-029E-9C41-8D1C-263771246F7D}">
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView topLeftCell="A2" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
+      <selection sqref="A1:N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -955,22 +1129,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19" t="s">
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
     </row>
     <row r="2" spans="1:14" ht="73" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1445,16 +1619,16 @@
       <c r="D18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
@@ -1463,13 +1637,13 @@
       <c r="B21" s="10"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
       <c r="F22" t="s">
         <v>27</v>
       </c>
@@ -1488,13 +1662,13 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
       <c r="F23" t="s">
         <v>27</v>
       </c>
@@ -1513,13 +1687,13 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
       <c r="F24" t="s">
         <v>27</v>
       </c>
@@ -1531,13 +1705,13 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
       <c r="J25" t="s">
         <v>96</v>
       </c>
@@ -1547,13 +1721,13 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
       <c r="J26" t="s">
         <v>96</v>
       </c>
@@ -1563,13 +1737,13 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
       <c r="J27" t="s">
         <v>96</v>
       </c>
@@ -1579,13 +1753,13 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
       <c r="J28" t="s">
         <v>96</v>
       </c>
@@ -1595,13 +1769,13 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
       <c r="J29" t="s">
         <v>96</v>
       </c>
@@ -1611,13 +1785,13 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
       <c r="J30" t="s">
         <v>96</v>
       </c>
@@ -1627,13 +1801,13 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
       <c r="J31" t="s">
         <v>96</v>
       </c>
@@ -1671,6 +1845,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="E18:N18"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A28:E28"/>
     <mergeCell ref="A29:E29"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="A31:E31"/>
@@ -1679,45 +1858,40 @@
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A27:E27"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="E18:N18"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A28:E28"/>
   </mergeCells>
   <conditionalFormatting sqref="C5 L12:N13 I9:N10 E5:N5 C12:J13 C14:N16 C9:G10 C11:N11 C6:N8">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:N10 C9:G10 C11:N16 C5:N8">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"o"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"o"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1727,6 +1901,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F2AC82D-6DE3-D44B-BAC0-41104FA573B4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C579E461-CCEA-AF4F-B470-CE30D12BD684}">
   <dimension ref="A1:D24"/>
   <sheetViews>
@@ -1865,17 +2054,577 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FFB997-BF08-CE43-A4D8-8F4B77EA4BDC}">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="N4" sqref="N3:N4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="26.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" style="22" customWidth="1"/>
+    <col min="3" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+    </row>
+    <row r="2" spans="1:13" s="22" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="25"/>
+      <c r="B2" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+    </row>
+    <row r="3" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="M4" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="J5" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="L5" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="J6" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="K6" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="L6" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="M6" s="29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="L7" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="M7" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="L8" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="M8" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="L9" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="M9" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="L10" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="M10" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I11" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="J11" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="M11" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I12" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="J12" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="K12" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="H13" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I13" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="J13" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="K13" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="L13" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="M13" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="102" x14ac:dyDescent="0.2">
+      <c r="A14" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="J1:M1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="84" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
🚧 (results): WIP - Re-plotting case study
</commit_message>
<xml_diff>
--- a/dissertation/designs/Heuristic Consolidation.xlsx
+++ b/dissertation/designs/Heuristic Consolidation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arneschreuder/Development/personal/masters.ai/dissertation/designs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6C019C-9CFD-7442-B847-2C68B05AF811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DFDC91-06B7-A74B-8E7B-E16365DBE5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{6DFA7F91-D994-1E45-B9E7-F07B16B402EA}"/>
   </bookViews>
@@ -2065,8 +2065,8 @@
   </sheetPr>
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="N4" sqref="N3:N4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
🚧 (article): Save point
</commit_message>
<xml_diff>
--- a/dissertation/designs/Heuristic Consolidation.xlsx
+++ b/dissertation/designs/Heuristic Consolidation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arneschreuder/Development/personal/masters.ai/dissertation/designs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arneschreuder/Development/Personal/masters.ai/dissertation/designs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DFDC91-06B7-A74B-8E7B-E16365DBE5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BBD4D9-155F-404E-9E0C-EF9FFEA036A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{6DFA7F91-D994-1E45-B9E7-F07B16B402EA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="3" xr2:uid="{6DFA7F91-D994-1E45-B9E7-F07B16B402EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -393,15 +396,9 @@
     <t>learning rate</t>
   </si>
   <si>
-    <t>learning rate, epsilon</t>
-  </si>
-  <si>
     <t>mutation rate</t>
   </si>
   <si>
-    <t xml:space="preserve">burn in, replay window size, population size, reselection and reanalysis window size, normalisation, discounted rewards  </t>
-  </si>
-  <si>
     <t>Population State</t>
   </si>
   <si>
@@ -420,25 +417,45 @@
     <t>Is analogous to velocity</t>
   </si>
   <si>
-    <t>learning rate, momentum (maps to hp1)</t>
-  </si>
-  <si>
     <t>expected gradient mean (hp1)</t>
   </si>
   <si>
     <t>expected gradient variance (hp2)</t>
   </si>
   <si>
-    <t>learning rate, rho  (maps to hp2), momentum (maps to hp1), epsilon</t>
-  </si>
-  <si>
-    <t>rho (maps to hp2), epsilon</t>
-  </si>
-  <si>
-    <t>learning rate, momentum (maps to hp1), rho (maps to hp2)</t>
-  </si>
-  <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>learning rate,
+momentum (maps to hp1)</t>
+  </si>
+  <si>
+    <t>learning rate,
+rho  (maps to hp2),
+momentum (maps to hp1),
+epsilon</t>
+  </si>
+  <si>
+    <t>rho (maps to hp2),
+epsilon</t>
+  </si>
+  <si>
+    <t>learning rate,
+momentum (maps to hp1),
+rho (maps to hp2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">burn in,
+replay window size,
+population size,
+reselection,
+reanalysis window size,
+normalisation,
+discounted rewards  </t>
+  </si>
+  <si>
+    <t>learning rate,
+epsilon</t>
   </si>
 </sst>
 </file>
@@ -547,7 +564,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -579,11 +596,103 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -627,6 +736,18 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -638,85 +759,62 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1129,22 +1227,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="20" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
     </row>
     <row r="2" spans="1:14" ht="73" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1619,16 +1717,16 @@
       <c r="D18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
@@ -1637,13 +1735,13 @@
       <c r="B21" s="10"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
       <c r="F22" t="s">
         <v>27</v>
       </c>
@@ -1662,13 +1760,13 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
       <c r="F23" t="s">
         <v>27</v>
       </c>
@@ -1687,13 +1785,13 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
       <c r="F24" t="s">
         <v>27</v>
       </c>
@@ -1705,13 +1803,13 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
       <c r="J25" t="s">
         <v>96</v>
       </c>
@@ -1721,13 +1819,13 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
       <c r="J26" t="s">
         <v>96</v>
       </c>
@@ -1737,13 +1835,13 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
       <c r="J27" t="s">
         <v>96</v>
       </c>
@@ -1753,13 +1851,13 @@
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
       <c r="J28" t="s">
         <v>96</v>
       </c>
@@ -1769,13 +1867,13 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
       <c r="J29" t="s">
         <v>96</v>
       </c>
@@ -1785,13 +1883,13 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
       <c r="J30" t="s">
         <v>96</v>
       </c>
@@ -1801,13 +1899,13 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
       <c r="J31" t="s">
         <v>96</v>
       </c>
@@ -1860,38 +1958,38 @@
     <mergeCell ref="A27:E27"/>
   </mergeCells>
   <conditionalFormatting sqref="C5 L12:N13 I9:N10 E5:N5 C12:J13 C14:N16 C9:G10 C11:N11 C6:N8">
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:N10 C9:G10 C11:N16 C5:N8">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"o"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"o"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2065,19 +2163,19 @@
   </sheetPr>
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection sqref="A1:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" customWidth="1"/>
-    <col min="7" max="7" width="13.5" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5" customWidth="1"/>
     <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.1640625" bestFit="1" customWidth="1"/>
@@ -2086,536 +2184,536 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24" t="s">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+    </row>
+    <row r="2" spans="1:13" s="18" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="20"/>
+      <c r="B2" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="30"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+    </row>
+    <row r="3" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-    </row>
-    <row r="2" spans="1:13" s="22" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="27" t="s">
+      <c r="C3" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2" s="27" t="s">
+      <c r="I3" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-    </row>
-    <row r="3" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="G3" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="H3" s="28" t="s">
+      <c r="J3" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="M4" s="27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="C5" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="K5" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="L5" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="42"/>
+      <c r="C6" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="J7" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="M7" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="J3" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="28" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="H4" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="I4" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="J4" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="K4" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="L4" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="M4" s="29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="H5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="K5" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="L5" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="M5" s="29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="G6" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="H6" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="J6" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="K6" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="L6" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="M6" s="29" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" s="25" t="s">
+      <c r="C8" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="L8" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="M8" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="L9" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="M9" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="L10" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="M10" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="J11" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="M11" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="42"/>
+      <c r="C12" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="J12" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="K12" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="M12" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="H7" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="I7" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="J7" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="K7" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="L7" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="M7" s="29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="H8" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="I8" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="K8" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="L8" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="M8" s="29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="G9" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="I9" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="K9" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="L9" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="M9" s="29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10" s="25" t="s">
+      <c r="C13" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="J13" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="K13" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="L13" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="M13" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="119" x14ac:dyDescent="0.2">
+      <c r="A14" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="C10" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="H10" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="K10" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="L10" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="M10" s="29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="H11" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="I11" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="J11" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="M11" s="29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="H12" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="I12" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="J12" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="K12" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="M12" s="29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="H13" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="I13" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="J13" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="K13" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="L13" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="M13" s="29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="102" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="L14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="M14" s="29" t="s">
+      <c r="C14" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" s="27" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2625,6 +2723,6 @@
     <mergeCell ref="J1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="84" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>